<commit_message>
Fixing bugs and change celery task
</commit_message>
<xml_diff>
--- a/admin/Menu.xlsx
+++ b/admin/Menu.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Job\Python_projects\FastAPI(Docker)\admin\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A1959E4F-E5FD-4F70-B017-1736E7E5C9D9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0C2AE54C-7322-400E-942C-F7F8267CFE24}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1920" yWindow="0" windowWidth="12468" windowHeight="12960" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -30,163 +30,163 @@
     <t>Меню</t>
   </si>
   <si>
+    <t>Холодные закуски</t>
+  </si>
+  <si>
+    <t>К пиву</t>
+  </si>
+  <si>
+    <t>Сельдь Бисмарк</t>
+  </si>
+  <si>
+    <t>Традиционное немецкое блюдо из маринованной сельди</t>
+  </si>
+  <si>
+    <t>Мясная тарелка</t>
+  </si>
+  <si>
+    <t>Рыбная тарелка</t>
+  </si>
+  <si>
+    <t>Нарезка из креветок, кальмаров, раковых шеек, гребешков, лосося, скумбрии и красной икры</t>
+  </si>
+  <si>
+    <t>Рамен</t>
+  </si>
+  <si>
+    <t>Горячий рамен</t>
+  </si>
+  <si>
+    <t>Дайзу рамен</t>
+  </si>
+  <si>
+    <t>Рамен на курином бульоне с куриными подушками и яйцом аджитама, яично-пшеничной лапшой, ростки зелени, грибами муэр и зеленым луком</t>
+  </si>
+  <si>
+    <t>Унаги рамен</t>
+  </si>
+  <si>
+    <t>Рамен на нежном сливочном рыбном бульоне, с добавлением маринованного угря, грибов муэр, кунжута, зеленого лука</t>
+  </si>
+  <si>
+    <t>Чиизу Рамен</t>
+  </si>
+  <si>
+    <t>Рамен на насыщенном сырном бульоне на основе кокосового молока, с добавлением куриной грудинки, яично - пшеничной лапши, мисо-матадоре, ростков зелени, листьев вакамэ</t>
+  </si>
+  <si>
+    <t>Алкогольное меню</t>
+  </si>
+  <si>
+    <t>Алкогольные напитки</t>
+  </si>
+  <si>
+    <t>Красные вина</t>
+  </si>
+  <si>
+    <t>Для романтичного вечера</t>
+  </si>
+  <si>
+    <t>Шемен де Пап ля Ноблесс</t>
+  </si>
+  <si>
+    <t>Вино красное — фруктовое, среднетелое, выдержанное в дубе</t>
+  </si>
+  <si>
+    <t>Рипароссо Монтепульчано</t>
+  </si>
+  <si>
+    <t>Вино красное, сухое</t>
+  </si>
+  <si>
+    <t>Кьянти, Серристори</t>
+  </si>
+  <si>
+    <t>Вино красное — элегантное, комплексное, не выдержанное в дубе</t>
+  </si>
+  <si>
+    <t>Виски</t>
+  </si>
+  <si>
+    <t>Для интересных бесед</t>
+  </si>
+  <si>
+    <t>Джемисон</t>
+  </si>
+  <si>
+    <t>Классический купажированный виски, проходящий 4-хлетнюю выдержку в дубовых бочках</t>
+  </si>
+  <si>
+    <t>Джек Дэниелс</t>
+  </si>
+  <si>
+    <t>Характерен мягкий вкус, сочетает в себе карамельно-ванильные и древесные нотки. Легкий привкус дыма.</t>
+  </si>
+  <si>
+    <t>Чивас Ригал</t>
+  </si>
+  <si>
+    <t>Это купаж высококачественных солодовых и зерновых виски, выдержанных как минимум в течение 12 лет, что придает напитку роскошные нотки меда, ванили и спелых яблок.</t>
+  </si>
+  <si>
+    <t>Нарезка из ветчины, колбасных колечек, нескольких сортов сыра и фруктов</t>
+  </si>
+  <si>
+    <t>9224469d-59a2-4932-867e-929f4eb0e0df</t>
+  </si>
+  <si>
+    <t>0acb58e5-21c2-499f-a4f2-eac14efa4d5d</t>
+  </si>
+  <si>
+    <t>032dce74-a930-4978-b7a8-b99295d0635d</t>
+  </si>
+  <si>
+    <t>6e2b3379-71fe-4559-9cae-1c3ae22c821d</t>
+  </si>
+  <si>
+    <t>1071ca81-8bcd-44eb-807e-7506e99abb1f</t>
+  </si>
+  <si>
+    <t>acbaa20d-d276-41cf-a55f-c928f3b81d15</t>
+  </si>
+  <si>
+    <t>fa46b7e4-b230-4b85-8463-e1ea0f2d18e6</t>
+  </si>
+  <si>
+    <t>e5c6f33b-6a59-43d9-a36b-408a6e47c932</t>
+  </si>
+  <si>
+    <t>f48e43d3-5d7a-4fb3-b5ca-3f4a226793f4</t>
+  </si>
+  <si>
+    <t>6b295851-f348-45f4-96a1-a24358f698c4</t>
+  </si>
+  <si>
+    <t>7eb36bbd-f8bb-4e25-9ca0-671bb26ba828</t>
+  </si>
+  <si>
+    <t>d09985df-ac4b-4676-89e6-6e89401da71d</t>
+  </si>
+  <si>
+    <t>c3be21f9-486b-4e8d-94b2-6cc08129416c</t>
+  </si>
+  <si>
+    <t>0c019fc0-c0e1-4145-95c2-5147da81c531</t>
+  </si>
+  <si>
+    <t>ce26c66a-2bfe-4690-a075-3c2c40133e26</t>
+  </si>
+  <si>
+    <t>684a39f2-ca42-41bb-93c2-0c396977ca65</t>
+  </si>
+  <si>
+    <t>beb7cb9a-ec10-4644-bda6-2c0f28b4595b</t>
+  </si>
+  <si>
+    <t>351f9e38-80e5-4085-aa0b-4847cc74246d</t>
+  </si>
+  <si>
     <t>Основное меню</t>
-  </si>
-  <si>
-    <t>Холодные закуски</t>
-  </si>
-  <si>
-    <t>К пиву</t>
-  </si>
-  <si>
-    <t>Сельдь Бисмарк</t>
-  </si>
-  <si>
-    <t>Традиционное немецкое блюдо из маринованной сельди</t>
-  </si>
-  <si>
-    <t>Мясная тарелка</t>
-  </si>
-  <si>
-    <t>Рыбная тарелка</t>
-  </si>
-  <si>
-    <t>Нарезка из креветок, кальмаров, раковых шеек, гребешков, лосося, скумбрии и красной икры</t>
-  </si>
-  <si>
-    <t>Рамен</t>
-  </si>
-  <si>
-    <t>Горячий рамен</t>
-  </si>
-  <si>
-    <t>Дайзу рамен</t>
-  </si>
-  <si>
-    <t>Рамен на курином бульоне с куриными подушками и яйцом аджитама, яично-пшеничной лапшой, ростки зелени, грибами муэр и зеленым луком</t>
-  </si>
-  <si>
-    <t>Унаги рамен</t>
-  </si>
-  <si>
-    <t>Рамен на нежном сливочном рыбном бульоне, с добавлением маринованного угря, грибов муэр, кунжута, зеленого лука</t>
-  </si>
-  <si>
-    <t>Чиизу Рамен</t>
-  </si>
-  <si>
-    <t>Рамен на насыщенном сырном бульоне на основе кокосового молока, с добавлением куриной грудинки, яично - пшеничной лапши, мисо-матадоре, ростков зелени, листьев вакамэ</t>
-  </si>
-  <si>
-    <t>Алкогольное меню</t>
-  </si>
-  <si>
-    <t>Алкогольные напитки</t>
-  </si>
-  <si>
-    <t>Красные вина</t>
-  </si>
-  <si>
-    <t>Для романтичного вечера</t>
-  </si>
-  <si>
-    <t>Шемен де Пап ля Ноблесс</t>
-  </si>
-  <si>
-    <t>Вино красное — фруктовое, среднетелое, выдержанное в дубе</t>
-  </si>
-  <si>
-    <t>Рипароссо Монтепульчано</t>
-  </si>
-  <si>
-    <t>Вино красное, сухое</t>
-  </si>
-  <si>
-    <t>Кьянти, Серристори</t>
-  </si>
-  <si>
-    <t>Вино красное — элегантное, комплексное, не выдержанное в дубе</t>
-  </si>
-  <si>
-    <t>Виски</t>
-  </si>
-  <si>
-    <t>Для интересных бесед</t>
-  </si>
-  <si>
-    <t>Джемисон</t>
-  </si>
-  <si>
-    <t>Классический купажированный виски, проходящий 4-хлетнюю выдержку в дубовых бочках</t>
-  </si>
-  <si>
-    <t>Джек Дэниелс</t>
-  </si>
-  <si>
-    <t>Характерен мягкий вкус, сочетает в себе карамельно-ванильные и древесные нотки. Легкий привкус дыма.</t>
-  </si>
-  <si>
-    <t>Чивас Ригал</t>
-  </si>
-  <si>
-    <t>Это купаж высококачественных солодовых и зерновых виски, выдержанных как минимум в течение 12 лет, что придает напитку роскошные нотки меда, ванили и спелых яблок.</t>
-  </si>
-  <si>
-    <t>Нарезка из ветчины, колбасных колечек, нескольких сортов сыра и фруктов</t>
-  </si>
-  <si>
-    <t>9224469d-59a2-4932-867e-929f4eb0e0df</t>
-  </si>
-  <si>
-    <t>0acb58e5-21c2-499f-a4f2-eac14efa4d5d</t>
-  </si>
-  <si>
-    <t>032dce74-a930-4978-b7a8-b99295d0635d</t>
-  </si>
-  <si>
-    <t>6e2b3379-71fe-4559-9cae-1c3ae22c821d</t>
-  </si>
-  <si>
-    <t>1071ca81-8bcd-44eb-807e-7506e99abb1f</t>
-  </si>
-  <si>
-    <t>acbaa20d-d276-41cf-a55f-c928f3b81d15</t>
-  </si>
-  <si>
-    <t>fa46b7e4-b230-4b85-8463-e1ea0f2d18e6</t>
-  </si>
-  <si>
-    <t>e5c6f33b-6a59-43d9-a36b-408a6e47c932</t>
-  </si>
-  <si>
-    <t>f48e43d3-5d7a-4fb3-b5ca-3f4a226793f4</t>
-  </si>
-  <si>
-    <t>6b295851-f348-45f4-96a1-a24358f698c4</t>
-  </si>
-  <si>
-    <t>7eb36bbd-f8bb-4e25-9ca0-671bb26ba828</t>
-  </si>
-  <si>
-    <t>d09985df-ac4b-4676-89e6-6e89401da71d</t>
-  </si>
-  <si>
-    <t>c3be21f9-486b-4e8d-94b2-6cc08129416c</t>
-  </si>
-  <si>
-    <t>0c019fc0-c0e1-4145-95c2-5147da81c531</t>
-  </si>
-  <si>
-    <t>ce26c66a-2bfe-4690-a075-3c2c40133e26</t>
-  </si>
-  <si>
-    <t>684a39f2-ca42-41bb-93c2-0c396977ca65</t>
-  </si>
-  <si>
-    <t>beb7cb9a-ec10-4644-bda6-2c0f28b4595b</t>
-  </si>
-  <si>
-    <t>351f9e38-80e5-4085-aa0b-4847cc74246d</t>
   </si>
 </sst>
 </file>
@@ -484,7 +484,7 @@
   <dimension ref="A1:F1000"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C21" sqref="C21"/>
+      <selection activeCell="E19" sqref="E19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5546875" defaultRowHeight="15" customHeight="1"/>
@@ -499,13 +499,13 @@
   <sheetData>
     <row r="1" spans="1:6" ht="15.75" customHeight="1">
       <c r="A1" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>1</v>
+        <v>53</v>
       </c>
       <c r="D1" s="8"/>
       <c r="E1" s="8"/>
@@ -514,13 +514,13 @@
     <row r="2" spans="1:6" ht="15.75" customHeight="1">
       <c r="A2" s="2"/>
       <c r="B2" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D2" s="8" t="s">
         <v>2</v>
-      </c>
-      <c r="D2" s="8" t="s">
-        <v>3</v>
       </c>
       <c r="E2" s="8"/>
       <c r="F2" s="2"/>
@@ -529,13 +529,13 @@
       <c r="A3" s="2"/>
       <c r="B3" s="1"/>
       <c r="C3" s="3" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D3" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="E3" s="7" t="s">
         <v>4</v>
-      </c>
-      <c r="E3" s="7" t="s">
-        <v>5</v>
       </c>
       <c r="F3" s="4">
         <v>182.99</v>
@@ -545,13 +545,13 @@
       <c r="A4" s="2"/>
       <c r="B4" s="1"/>
       <c r="C4" s="3" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D4" s="8" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E4" s="6" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="F4" s="4">
         <v>215.36</v>
@@ -561,13 +561,13 @@
       <c r="A5" s="2"/>
       <c r="B5" s="1"/>
       <c r="C5" s="3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D5" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="E5" s="7" t="s">
         <v>7</v>
-      </c>
-      <c r="E5" s="7" t="s">
-        <v>8</v>
       </c>
       <c r="F5" s="4">
         <v>265.57</v>
@@ -576,13 +576,13 @@
     <row r="6" spans="1:6" ht="15.75" customHeight="1">
       <c r="A6" s="2"/>
       <c r="B6" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C6" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D6" s="8" t="s">
         <v>9</v>
-      </c>
-      <c r="D6" s="8" t="s">
-        <v>10</v>
       </c>
       <c r="E6" s="7"/>
       <c r="F6" s="2"/>
@@ -591,13 +591,13 @@
       <c r="A7" s="2"/>
       <c r="B7" s="2"/>
       <c r="C7" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D7" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="E7" s="7" t="s">
         <v>11</v>
-      </c>
-      <c r="E7" s="7" t="s">
-        <v>12</v>
       </c>
       <c r="F7" s="1">
         <v>166.47</v>
@@ -607,13 +607,13 @@
       <c r="A8" s="2"/>
       <c r="B8" s="2"/>
       <c r="C8" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D8" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="E8" s="7" t="s">
         <v>13</v>
-      </c>
-      <c r="E8" s="7" t="s">
-        <v>14</v>
       </c>
       <c r="F8" s="1">
         <v>168.25</v>
@@ -623,13 +623,13 @@
       <c r="A9" s="2"/>
       <c r="B9" s="2"/>
       <c r="C9" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D9" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="E9" s="7" t="s">
         <v>15</v>
-      </c>
-      <c r="E9" s="7" t="s">
-        <v>16</v>
       </c>
       <c r="F9" s="1">
         <v>132.88</v>
@@ -637,13 +637,13 @@
     </row>
     <row r="10" spans="1:6" ht="15.75" customHeight="1">
       <c r="A10" s="5" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B10" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C10" s="1" t="s">
         <v>17</v>
-      </c>
-      <c r="C10" s="1" t="s">
-        <v>18</v>
       </c>
       <c r="D10" s="8"/>
       <c r="E10" s="7"/>
@@ -652,13 +652,13 @@
     <row r="11" spans="1:6" ht="15.75" customHeight="1">
       <c r="A11" s="2"/>
       <c r="B11" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C11" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D11" s="8" t="s">
         <v>19</v>
-      </c>
-      <c r="D11" s="8" t="s">
-        <v>20</v>
       </c>
       <c r="E11" s="7"/>
       <c r="F11" s="2"/>
@@ -667,13 +667,13 @@
       <c r="A12" s="2"/>
       <c r="B12" s="1"/>
       <c r="C12" s="3" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D12" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="E12" s="7" t="s">
         <v>21</v>
-      </c>
-      <c r="E12" s="7" t="s">
-        <v>22</v>
       </c>
       <c r="F12" s="1">
         <v>2700.79</v>
@@ -683,13 +683,13 @@
       <c r="A13" s="2"/>
       <c r="B13" s="1"/>
       <c r="C13" s="3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D13" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="E13" s="7" t="s">
         <v>23</v>
-      </c>
-      <c r="E13" s="7" t="s">
-        <v>24</v>
       </c>
       <c r="F13" s="1">
         <v>3100.33</v>
@@ -699,13 +699,13 @@
       <c r="A14" s="2"/>
       <c r="B14" s="1"/>
       <c r="C14" s="3" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D14" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="E14" s="7" t="s">
         <v>25</v>
-      </c>
-      <c r="E14" s="7" t="s">
-        <v>26</v>
       </c>
       <c r="F14" s="1">
         <v>1850.42</v>
@@ -714,13 +714,13 @@
     <row r="15" spans="1:6" ht="15.75" customHeight="1">
       <c r="A15" s="2"/>
       <c r="B15" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C15" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="D15" s="8" t="s">
         <v>27</v>
-      </c>
-      <c r="D15" s="8" t="s">
-        <v>28</v>
       </c>
       <c r="E15" s="7"/>
       <c r="F15" s="2"/>
@@ -729,13 +729,13 @@
       <c r="A16" s="2"/>
       <c r="B16" s="2"/>
       <c r="C16" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D16" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="E16" s="7" t="s">
         <v>29</v>
-      </c>
-      <c r="E16" s="7" t="s">
-        <v>30</v>
       </c>
       <c r="F16" s="1">
         <v>420.78</v>
@@ -745,13 +745,13 @@
       <c r="A17" s="2"/>
       <c r="B17" s="2"/>
       <c r="C17" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D17" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="E17" s="7" t="s">
         <v>31</v>
-      </c>
-      <c r="E17" s="7" t="s">
-        <v>32</v>
       </c>
       <c r="F17" s="1">
         <v>440.11</v>
@@ -761,13 +761,13 @@
       <c r="A18" s="2"/>
       <c r="B18" s="2"/>
       <c r="C18" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D18" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="E18" s="7" t="s">
         <v>33</v>
-      </c>
-      <c r="E18" s="7" t="s">
-        <v>34</v>
       </c>
       <c r="F18" s="1">
         <v>520.08000000000004</v>

</xml_diff>